<commit_message>
Added ISBN 10 => 13 conversion function
</commit_message>
<xml_diff>
--- a/book_log.xlsx
+++ b/book_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ISBN</t>
   </si>
@@ -34,31 +34,13 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Dohrn, Bernardine</t>
-  </si>
-  <si>
-    <t>Lemert, Charles</t>
-  </si>
-  <si>
     <t>Schwartz, Morrie</t>
   </si>
   <si>
-    <t>Seven Stories Press</t>
-  </si>
-  <si>
-    <t>Westview Press</t>
-  </si>
-  <si>
     <t>Delta</t>
   </si>
   <si>
-    <t>Sing a Battle Song</t>
-  </si>
-  <si>
-    <t>Sociology after the crisis</t>
-  </si>
-  <si>
-    <t>Morrie</t>
+    <t>Morrie: In His Own Words</t>
   </si>
 </sst>
 </file>
@@ -416,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,62 +426,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>9781583227268</v>
+        <v>9780385318792</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>19.95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>9780813325446</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>9780813325446</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>385318790</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>15.6</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>